<commit_message>
Changed mulligans drawn method
</commit_message>
<xml_diff>
--- a/PokemonTCGSim/PrizeTest.xlsx
+++ b/PokemonTCGSim/PrizeTest.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Downloads\Programming Classes\eclipse-workspace\PokemonTCGSim\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\git\StatsProject1\PokemonTCGSim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E16386-36E3-4009-A16D-16D4A881CC51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F6883F-A0C4-4EF6-8E84-70A42D46E04A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{912F8785-0EC0-4B00-A90B-F3AB49694A39}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.00000"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -520,7 +520,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -960,7 +960,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00000" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1963,7 +1963,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>